<commit_message>
updating analysis after correcting policy dates
</commit_message>
<xml_diff>
--- a/data/tabled3.xlsx
+++ b/data/tabled3.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://drexel0-my.sharepoint.com/personal/as5494_drexel_edu/Documents/Alina Research/Research/Preemption and covid/covid_preemption_1/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="115" documentId="8_{DD7CA772-477F-D246-81F0-54C8D4C325DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2FA416CF-2DA8-4533-B65A-C5A822941DB9}"/>
+  <xr:revisionPtr revIDLastSave="164" documentId="8_{DD7CA772-477F-D246-81F0-54C8D4C325DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5202AE87-3062-4412-9875-CB5106990CA4}"/>
   <bookViews>
-    <workbookView xWindow="732" yWindow="732" windowWidth="13824" windowHeight="7176" xr2:uid="{7C621906-8E95-E248-9AC9-4885AC5EF2EC}"/>
+    <workbookView xWindow="11424" yWindow="444" windowWidth="19332" windowHeight="11028" xr2:uid="{7C621906-8E95-E248-9AC9-4885AC5EF2EC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -51,218 +51,175 @@
     <t>Alternative Specification 2</t>
   </si>
   <si>
-    <r>
-      <t>9.52</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>(4.87, 18.60)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>15.16</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>(9.69, 23.73)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>7.35</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>(3.47, 15.57)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve"> 11.58</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>(6.24, 21.49)</t>
-    </r>
-  </si>
-  <si>
-    <t>0.68(0.41, 1.11)</t>
-  </si>
-  <si>
-    <t>0.60(0.35, 1.03)</t>
-  </si>
-  <si>
-    <t>0.63(0.82, 1.21)</t>
-  </si>
-  <si>
-    <t>0.91(0.55, 1.50)</t>
-  </si>
-  <si>
-    <t>0.88(0.52, 1.49)</t>
-  </si>
-  <si>
-    <t>0.85(0.48, 1.50)</t>
-  </si>
-  <si>
-    <t>1.02(0.87, 1.19)</t>
-  </si>
-  <si>
-    <t>1.018(0.87, 1.18)</t>
-  </si>
-  <si>
-    <t>1.0(0.82, 1.20)</t>
-  </si>
-  <si>
-    <t>1.28(0.92, 1.79)</t>
-  </si>
-  <si>
-    <t>1.24(0.91, 1.67)</t>
-  </si>
-  <si>
-    <t>1.38(0.95, 2.0)</t>
-  </si>
-  <si>
-    <t>1.25(0.69, 2.24)</t>
-  </si>
-  <si>
-    <t>1.21(0.71, 2.06)</t>
-  </si>
-  <si>
-    <t>1.38(0.72, 2.63)</t>
-  </si>
-  <si>
-    <t>1.30(0.49, 3.43)</t>
-  </si>
-  <si>
-    <t>1.14(0.46, 2.82)</t>
-  </si>
-  <si>
-    <t>1.58(0.74, 3.37)</t>
-  </si>
-  <si>
-    <t>1.95(0.69, 5.51)</t>
-  </si>
-  <si>
-    <t>1.35(0.38, 4.80)</t>
-  </si>
-  <si>
-    <t>1.63(0.44, 6.00)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  3.22(0.99, 10.47)</t>
-  </si>
-  <si>
-    <t>2.59(0.79, 8.46)</t>
-  </si>
-  <si>
-    <t>2.74(0.94, 7.98)</t>
-  </si>
-  <si>
-    <t>5.09(1.52, 17.05)</t>
-  </si>
-  <si>
-    <t>4.0(1.23, 13.35)</t>
-  </si>
-  <si>
-    <t>3.59(1.27, 10.16)</t>
-  </si>
-  <si>
-    <t>7.56(2.17, 26.37)</t>
-  </si>
-  <si>
-    <t>6.00(1.62, 22.22)</t>
-  </si>
-  <si>
-    <t>5.0(1.61, 15.48)</t>
-  </si>
-  <si>
-    <t>12.98(4.26, 39.53)</t>
-  </si>
-  <si>
-    <t>9.73(2.97, 34.84)</t>
-  </si>
-  <si>
-    <t>8.73(3.18, 23.97)</t>
-  </si>
-  <si>
-    <t>11.14(4.41, 28.17))</t>
-  </si>
-  <si>
-    <t>11.34(5.26, 24.47)</t>
-  </si>
-  <si>
-    <t>11.08(5.08, 24.14)</t>
-  </si>
-  <si>
-    <t>14.07(7.22, 27.40)</t>
+    <t>0.53 
+(0.31, 0.91)</t>
+  </si>
+  <si>
+    <t>0.80
+ (0.47, 1.38)</t>
+  </si>
+  <si>
+    <t>0.99
+(0.83, 1.20)</t>
+  </si>
+  <si>
+    <t>1.28
+ (0.94, 1.75)</t>
+  </si>
+  <si>
+    <t>1.40
+ (0.84, 2.31)</t>
+  </si>
+  <si>
+    <t>1.78 
+(0.87, 3.65)</t>
+  </si>
+  <si>
+    <t>2.82 
+(0.89, 8.88)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  4.69
+ (1.52, 14.44)</t>
+  </si>
+  <si>
+    <t>7.94
+ (2.36, 26.7)</t>
+  </si>
+  <si>
+    <t>9.88
+ (3.08, 31.65)</t>
+  </si>
+  <si>
+    <t>15.35
+ (5.35, 44.05)</t>
+  </si>
+  <si>
+    <t>0.45 
+(0.24, 0.85)</t>
+  </si>
+  <si>
+    <t>0.76
+ (0.41, 1.37)</t>
+  </si>
+  <si>
+    <t>0.98 
+(0.80, 1.20)</t>
+  </si>
+  <si>
+    <t>1.26 
+(0.92, 1.74)</t>
+  </si>
+  <si>
+    <t>1.45 
+(0.86, 2.43)</t>
+  </si>
+  <si>
+    <t>1.72 
+(0.79, 3.74)</t>
+  </si>
+  <si>
+    <t>2.65 
+(0.79, 8.86)</t>
+  </si>
+  <si>
+    <t>4.3 
+(1.36, 13.64)</t>
+  </si>
+  <si>
+    <t>6.93
+(2.00, 24.02)</t>
+  </si>
+  <si>
+    <t>8.71 
+(2.52, 30.11)</t>
+  </si>
+  <si>
+    <t>13.57 
+(4.34, 42.37)</t>
+  </si>
+  <si>
+    <t>13.54
+(5.60, 32.72)</t>
+  </si>
+  <si>
+    <t>14.45
+ (6.03, 34.63)</t>
+  </si>
+  <si>
+    <t>12.84 
+(5.70, 28.93)</t>
+  </si>
+  <si>
+    <t>11.06
+ (4.91, 24.88)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 10.63
+(5.65, 19.98)</t>
+  </si>
+  <si>
+    <t>12.83
+(7.07, 23.28)</t>
+  </si>
+  <si>
+    <t>13.24
+(6.06, 28.89)</t>
+  </si>
+  <si>
+    <t>12.03 
+(5.20, 27.84)</t>
+  </si>
+  <si>
+    <t>12.68 
+(4.15, 38.78)</t>
+  </si>
+  <si>
+    <t>8.52 
+(2.43, 29.85)</t>
+  </si>
+  <si>
+    <t>6.99 
+(2.01, 24.34)</t>
+  </si>
+  <si>
+    <t>4.5 
+(1.38, 14.64)</t>
+  </si>
+  <si>
+    <t>2.94 
+(0.99, 8.75)</t>
+  </si>
+  <si>
+    <t>1.89 
+(0.88, 4.05)</t>
+  </si>
+  <si>
+    <t>1.37 
+(0.77, 2.44)</t>
+  </si>
+  <si>
+    <t>1.29 
+(0.93, 1.80)</t>
+  </si>
+  <si>
+    <t>0.98 
+(0.81, 1.19)</t>
+  </si>
+  <si>
+    <t>0.78 
+(0.44, 1.38)</t>
+  </si>
+  <si>
+    <t>0.50 
+(0.28, 0.88)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -284,13 +241,6 @@
       <family val="1"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <vertAlign val="superscript"/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
@@ -393,7 +343,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -718,8 +668,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B646BB4-4C94-5640-9F7B-F407FEC9742B}">
   <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -743,13 +693,13 @@
         <v>-4</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>11</v>
+        <v>45</v>
       </c>
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
@@ -759,13 +709,13 @@
         <v>-3</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>14</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="37.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -773,13 +723,13 @@
         <v>-2</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>17</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -801,13 +751,13 @@
         <v>1</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>19</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -815,13 +765,13 @@
         <v>2</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>23</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -829,13 +779,13 @@
         <v>3</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -843,13 +793,13 @@
         <v>4</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -857,13 +807,13 @@
         <v>5</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -871,13 +821,13 @@
         <v>6</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>33</v>
+        <v>13</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -885,13 +835,13 @@
         <v>7</v>
       </c>
       <c r="B12" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" s="4" t="s">
         <v>36</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -899,13 +849,13 @@
         <v>8</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>39</v>
+        <v>15</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -914,10 +864,10 @@
       </c>
       <c r="B14" s="3"/>
       <c r="C14" s="3" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -926,34 +876,34 @@
       </c>
       <c r="B15" s="3"/>
       <c r="C15" s="8" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="31.2" thickBot="1" x14ac:dyDescent="0.35">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="3">
         <v>11</v>
       </c>
       <c r="B16" s="3"/>
       <c r="C16" s="3" t="s">
-        <v>5</v>
+        <v>29</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="31.2" thickBot="1" x14ac:dyDescent="0.35">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="3">
         <v>12</v>
       </c>
       <c r="B17" s="3"/>
       <c r="C17" s="3" t="s">
-        <v>7</v>
+        <v>30</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>